<commit_message>
update sd settings: tank heigh to meters instead of centimeters
</commit_message>
<xml_diff>
--- a/4-3782/sd/sd.xlsx
+++ b/4-3782/sd/sd.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kordianpiduch/Desktop/proj/sd/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kordianpiduch/Desktop/4-3782/sd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4B2F3F-9713-6E4F-93C7-023B6C70532D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B859E25-7FD2-7B4C-BE80-255DF37BA054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30080" windowHeight="32120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30080" windowHeight="32120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valves" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,19 @@
     <sheet name="drafts" sheetId="4" r:id="rId4"/>
     <sheet name="deflections" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1881,8 +1893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1964,7 +1976,7 @@
         <v>72</v>
       </c>
       <c r="J2">
-        <v>2097.5</v>
+        <v>20.975000000000001</v>
       </c>
       <c r="K2" t="s">
         <v>73</v>
@@ -2008,7 +2020,7 @@
         <v>72</v>
       </c>
       <c r="J3">
-        <v>2097.5</v>
+        <v>20.975000000000001</v>
       </c>
       <c r="K3" t="s">
         <v>73</v>
@@ -2052,7 +2064,7 @@
         <v>72</v>
       </c>
       <c r="J4">
-        <v>2097.5</v>
+        <v>20.975000000000001</v>
       </c>
       <c r="K4" t="s">
         <v>73</v>
@@ -2096,7 +2108,7 @@
         <v>72</v>
       </c>
       <c r="J5">
-        <v>2097.5</v>
+        <v>20.975000000000001</v>
       </c>
       <c r="K5" t="s">
         <v>73</v>
@@ -2140,7 +2152,7 @@
         <v>72</v>
       </c>
       <c r="J6">
-        <v>2097.5</v>
+        <v>20.975000000000001</v>
       </c>
       <c r="K6" t="s">
         <v>73</v>
@@ -2184,7 +2196,7 @@
         <v>72</v>
       </c>
       <c r="J7">
-        <v>2097.5</v>
+        <v>20.975000000000001</v>
       </c>
       <c r="K7" t="s">
         <v>73</v>
@@ -2228,7 +2240,7 @@
         <v>72</v>
       </c>
       <c r="J8">
-        <v>2097.5</v>
+        <v>20.975000000000001</v>
       </c>
       <c r="K8" t="s">
         <v>73</v>
@@ -2272,7 +2284,7 @@
         <v>72</v>
       </c>
       <c r="J9">
-        <v>2097.5</v>
+        <v>20.975000000000001</v>
       </c>
       <c r="K9" t="s">
         <v>73</v>
@@ -2316,7 +2328,7 @@
         <v>72</v>
       </c>
       <c r="J10">
-        <v>761.9</v>
+        <v>7.6189999999999998</v>
       </c>
       <c r="K10" t="s">
         <v>73</v>
@@ -2360,7 +2372,7 @@
         <v>72</v>
       </c>
       <c r="J11">
-        <v>761.9</v>
+        <v>7.6189999999999998</v>
       </c>
       <c r="K11" t="s">
         <v>73</v>
@@ -2404,7 +2416,7 @@
         <v>72</v>
       </c>
       <c r="J12">
-        <v>930</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="K12" t="s">
         <v>73</v>
@@ -2448,7 +2460,7 @@
         <v>72</v>
       </c>
       <c r="J13">
-        <v>618.9</v>
+        <v>6.1890000000000001</v>
       </c>
       <c r="K13" t="s">
         <v>73</v>
@@ -2492,7 +2504,7 @@
         <v>72</v>
       </c>
       <c r="J14">
-        <v>475.2</v>
+        <v>4.7519999999999998</v>
       </c>
       <c r="K14" t="s">
         <v>73</v>
@@ -2536,7 +2548,7 @@
         <v>72</v>
       </c>
       <c r="J15">
-        <v>475.2</v>
+        <v>4.7519999999999998</v>
       </c>
       <c r="K15" t="s">
         <v>73</v>
@@ -2580,7 +2592,7 @@
         <v>72</v>
       </c>
       <c r="J16">
-        <v>475.2</v>
+        <v>4.7519999999999998</v>
       </c>
       <c r="K16" t="s">
         <v>73</v>
@@ -2624,7 +2636,7 @@
         <v>72</v>
       </c>
       <c r="J17">
-        <v>621</v>
+        <v>6.21</v>
       </c>
       <c r="K17" t="s">
         <v>73</v>
@@ -2668,7 +2680,7 @@
         <v>72</v>
       </c>
       <c r="J18">
-        <v>495</v>
+        <v>4.95</v>
       </c>
       <c r="K18" t="s">
         <v>73</v>
@@ -2712,7 +2724,7 @@
         <v>72</v>
       </c>
       <c r="J19">
-        <v>525</v>
+        <v>5.25</v>
       </c>
       <c r="K19" t="s">
         <v>73</v>
@@ -2756,7 +2768,7 @@
         <v>72</v>
       </c>
       <c r="J20">
-        <v>525</v>
+        <v>5.25</v>
       </c>
       <c r="K20" t="s">
         <v>73</v>
@@ -2800,7 +2812,7 @@
         <v>72</v>
       </c>
       <c r="J21">
-        <v>525</v>
+        <v>5.25</v>
       </c>
       <c r="K21" t="s">
         <v>73</v>
@@ -2844,7 +2856,7 @@
         <v>72</v>
       </c>
       <c r="J22">
-        <v>525</v>
+        <v>5.25</v>
       </c>
       <c r="K22" t="s">
         <v>73</v>
@@ -2888,7 +2900,7 @@
         <v>72</v>
       </c>
       <c r="J23">
-        <v>236</v>
+        <v>2.36</v>
       </c>
       <c r="K23" t="s">
         <v>73</v>
@@ -2932,7 +2944,7 @@
         <v>72</v>
       </c>
       <c r="J24">
-        <v>236</v>
+        <v>2.36</v>
       </c>
       <c r="K24" t="s">
         <v>73</v>
@@ -2976,7 +2988,7 @@
         <v>72</v>
       </c>
       <c r="J25">
-        <v>1105</v>
+        <v>11.05</v>
       </c>
       <c r="K25" t="s">
         <v>73</v>
@@ -3020,7 +3032,7 @@
         <v>72</v>
       </c>
       <c r="J26">
-        <v>610</v>
+        <v>6.1</v>
       </c>
       <c r="K26" t="s">
         <v>73</v>
@@ -3064,7 +3076,7 @@
         <v>72</v>
       </c>
       <c r="J27">
-        <v>345</v>
+        <v>3.45</v>
       </c>
       <c r="K27" t="s">
         <v>73</v>
@@ -3108,7 +3120,7 @@
         <v>72</v>
       </c>
       <c r="J28">
-        <v>640</v>
+        <v>6.4</v>
       </c>
       <c r="K28" t="s">
         <v>73</v>
@@ -3152,7 +3164,7 @@
         <v>72</v>
       </c>
       <c r="J29">
-        <v>640</v>
+        <v>6.4</v>
       </c>
       <c r="K29" t="s">
         <v>73</v>
@@ -3279,8 +3291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3316,7 +3328,7 @@
         <v>133</v>
       </c>
       <c r="C2">
-        <v>1450</v>
+        <v>14.5</v>
       </c>
       <c r="D2" t="s">
         <v>68</v>
@@ -3339,7 +3351,7 @@
         <v>136</v>
       </c>
       <c r="C3">
-        <v>1450</v>
+        <v>14.5</v>
       </c>
       <c r="D3" t="s">
         <v>68</v>
@@ -3362,7 +3374,7 @@
         <v>138</v>
       </c>
       <c r="C4">
-        <v>1450</v>
+        <v>14.5</v>
       </c>
       <c r="D4" t="s">
         <v>68</v>
@@ -3385,7 +3397,7 @@
         <v>140</v>
       </c>
       <c r="C5">
-        <v>1450</v>
+        <v>14.5</v>
       </c>
       <c r="D5" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
update sd card settings
</commit_message>
<xml_diff>
--- a/4-3782/sd/sd.xlsx
+++ b/4-3782/sd/sd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kordianpiduch/Desktop/4-3782/sd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE19F2A-D5E3-2548-BE28-E4FAD3968039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A32F66A0-8316-BF4C-A2CE-5EB7E7303F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30080" windowHeight="32120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="37540" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valves" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="233">
   <si>
     <t>filename</t>
   </si>
@@ -1106,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1917,14 +1917,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="26.83203125" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" customWidth="1"/>
     <col min="10" max="10" width="21.5" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
@@ -1979,7 +1985,7 @@
         <v>202</v>
       </c>
       <c r="C2">
-        <v>999</v>
+        <v>1307.7</v>
       </c>
       <c r="D2" t="s">
         <v>68</v>
@@ -1987,8 +1993,8 @@
       <c r="E2" t="s">
         <v>69</v>
       </c>
-      <c r="F2" t="s">
-        <v>70</v>
+      <c r="F2">
+        <v>10</v>
       </c>
       <c r="G2" t="s">
         <v>71</v>
@@ -2023,7 +2029,7 @@
         <v>203</v>
       </c>
       <c r="C3">
-        <v>999</v>
+        <v>1307.7</v>
       </c>
       <c r="D3" t="s">
         <v>68</v>
@@ -2031,8 +2037,8 @@
       <c r="E3" t="s">
         <v>69</v>
       </c>
-      <c r="F3" t="s">
-        <v>70</v>
+      <c r="F3">
+        <v>10</v>
       </c>
       <c r="G3" t="s">
         <v>71</v>
@@ -2067,7 +2073,7 @@
         <v>204</v>
       </c>
       <c r="C4">
-        <v>999</v>
+        <v>1737.6</v>
       </c>
       <c r="D4" t="s">
         <v>68</v>
@@ -2075,8 +2081,8 @@
       <c r="E4" t="s">
         <v>69</v>
       </c>
-      <c r="F4" t="s">
-        <v>70</v>
+      <c r="F4">
+        <v>10</v>
       </c>
       <c r="G4" t="s">
         <v>71</v>
@@ -2111,7 +2117,7 @@
         <v>205</v>
       </c>
       <c r="C5">
-        <v>999</v>
+        <v>1737.6</v>
       </c>
       <c r="D5" t="s">
         <v>68</v>
@@ -2119,8 +2125,8 @@
       <c r="E5" t="s">
         <v>69</v>
       </c>
-      <c r="F5" t="s">
-        <v>70</v>
+      <c r="F5">
+        <v>10</v>
       </c>
       <c r="G5" t="s">
         <v>71</v>
@@ -2155,7 +2161,7 @@
         <v>206</v>
       </c>
       <c r="C6">
-        <v>999</v>
+        <v>3169.1</v>
       </c>
       <c r="D6" t="s">
         <v>68</v>
@@ -2163,8 +2169,8 @@
       <c r="E6" t="s">
         <v>69</v>
       </c>
-      <c r="F6" t="s">
-        <v>70</v>
+      <c r="F6">
+        <v>10</v>
       </c>
       <c r="G6" t="s">
         <v>71</v>
@@ -2199,7 +2205,7 @@
         <v>207</v>
       </c>
       <c r="C7">
-        <v>999</v>
+        <v>3169.1</v>
       </c>
       <c r="D7" t="s">
         <v>68</v>
@@ -2207,8 +2213,8 @@
       <c r="E7" t="s">
         <v>69</v>
       </c>
-      <c r="F7" t="s">
-        <v>70</v>
+      <c r="F7">
+        <v>10</v>
       </c>
       <c r="G7" t="s">
         <v>71</v>
@@ -2243,7 +2249,7 @@
         <v>208</v>
       </c>
       <c r="C8">
-        <v>999</v>
+        <v>3149.6</v>
       </c>
       <c r="D8" t="s">
         <v>68</v>
@@ -2251,8 +2257,8 @@
       <c r="E8" t="s">
         <v>69</v>
       </c>
-      <c r="F8" t="s">
-        <v>70</v>
+      <c r="F8">
+        <v>10</v>
       </c>
       <c r="G8" t="s">
         <v>71</v>
@@ -2287,7 +2293,7 @@
         <v>209</v>
       </c>
       <c r="C9">
-        <v>999</v>
+        <v>3222.9</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
@@ -2295,8 +2301,8 @@
       <c r="E9" t="s">
         <v>69</v>
       </c>
-      <c r="F9" t="s">
-        <v>70</v>
+      <c r="F9">
+        <v>10</v>
       </c>
       <c r="G9" t="s">
         <v>71</v>
@@ -2331,7 +2337,7 @@
         <v>210</v>
       </c>
       <c r="C10">
-        <v>999</v>
+        <v>839.5</v>
       </c>
       <c r="D10" t="s">
         <v>68</v>
@@ -2339,8 +2345,8 @@
       <c r="E10" t="s">
         <v>69</v>
       </c>
-      <c r="F10" t="s">
-        <v>70</v>
+      <c r="F10">
+        <v>10</v>
       </c>
       <c r="G10" t="s">
         <v>71</v>
@@ -2375,7 +2381,7 @@
         <v>211</v>
       </c>
       <c r="C11">
-        <v>999</v>
+        <v>839.5</v>
       </c>
       <c r="D11" t="s">
         <v>68</v>
@@ -2383,8 +2389,8 @@
       <c r="E11" t="s">
         <v>69</v>
       </c>
-      <c r="F11" t="s">
-        <v>70</v>
+      <c r="F11">
+        <v>10</v>
       </c>
       <c r="G11" t="s">
         <v>71</v>
@@ -2419,7 +2425,7 @@
         <v>212</v>
       </c>
       <c r="C12">
-        <v>999</v>
+        <v>1508.4</v>
       </c>
       <c r="D12" t="s">
         <v>68</v>
@@ -2427,8 +2433,8 @@
       <c r="E12" t="s">
         <v>69</v>
       </c>
-      <c r="F12" t="s">
-        <v>70</v>
+      <c r="F12">
+        <v>10</v>
       </c>
       <c r="G12" t="s">
         <v>71</v>
@@ -2463,7 +2469,7 @@
         <v>213</v>
       </c>
       <c r="C13">
-        <v>999</v>
+        <v>661.7</v>
       </c>
       <c r="D13" t="s">
         <v>68</v>
@@ -2471,8 +2477,8 @@
       <c r="E13" t="s">
         <v>69</v>
       </c>
-      <c r="F13" t="s">
-        <v>70</v>
+      <c r="F13">
+        <v>10</v>
       </c>
       <c r="G13" t="s">
         <v>71</v>
@@ -2507,7 +2513,7 @@
         <v>214</v>
       </c>
       <c r="C14">
-        <v>999</v>
+        <v>396.5</v>
       </c>
       <c r="D14" t="s">
         <v>86</v>
@@ -2515,8 +2521,8 @@
       <c r="E14" t="s">
         <v>69</v>
       </c>
-      <c r="F14" t="s">
-        <v>70</v>
+      <c r="F14">
+        <v>10</v>
       </c>
       <c r="G14" t="s">
         <v>71</v>
@@ -2551,7 +2557,7 @@
         <v>215</v>
       </c>
       <c r="C15">
-        <v>999</v>
+        <v>631.29999999999995</v>
       </c>
       <c r="D15" t="s">
         <v>86</v>
@@ -2559,8 +2565,8 @@
       <c r="E15" t="s">
         <v>69</v>
       </c>
-      <c r="F15" t="s">
-        <v>70</v>
+      <c r="F15">
+        <v>10</v>
       </c>
       <c r="G15" t="s">
         <v>71</v>
@@ -2595,7 +2601,7 @@
         <v>216</v>
       </c>
       <c r="C16">
-        <v>999</v>
+        <v>308.2</v>
       </c>
       <c r="D16" t="s">
         <v>86</v>
@@ -2603,8 +2609,8 @@
       <c r="E16" t="s">
         <v>69</v>
       </c>
-      <c r="F16" t="s">
-        <v>70</v>
+      <c r="F16">
+        <v>10</v>
       </c>
       <c r="G16" t="s">
         <v>71</v>
@@ -2639,7 +2645,7 @@
         <v>217</v>
       </c>
       <c r="C17">
-        <v>999</v>
+        <v>367.3</v>
       </c>
       <c r="D17" t="s">
         <v>86</v>
@@ -2647,8 +2653,8 @@
       <c r="E17" t="s">
         <v>69</v>
       </c>
-      <c r="F17" t="s">
-        <v>70</v>
+      <c r="F17">
+        <v>10</v>
       </c>
       <c r="G17" t="s">
         <v>71</v>
@@ -2683,7 +2689,7 @@
         <v>218</v>
       </c>
       <c r="C18">
-        <v>999</v>
+        <v>264.39999999999998</v>
       </c>
       <c r="D18" t="s">
         <v>86</v>
@@ -2691,8 +2697,8 @@
       <c r="E18" t="s">
         <v>69</v>
       </c>
-      <c r="F18" t="s">
-        <v>70</v>
+      <c r="F18">
+        <v>10</v>
       </c>
       <c r="G18" t="s">
         <v>71</v>
@@ -2727,7 +2733,7 @@
         <v>229</v>
       </c>
       <c r="C19">
-        <v>999</v>
+        <v>24.2</v>
       </c>
       <c r="D19" t="s">
         <v>86</v>
@@ -2735,8 +2741,8 @@
       <c r="E19" t="s">
         <v>69</v>
       </c>
-      <c r="F19" t="s">
-        <v>70</v>
+      <c r="F19">
+        <v>10</v>
       </c>
       <c r="G19" t="s">
         <v>71</v>
@@ -2771,7 +2777,7 @@
         <v>230</v>
       </c>
       <c r="C20">
-        <v>999</v>
+        <v>24.2</v>
       </c>
       <c r="D20" t="s">
         <v>86</v>
@@ -2779,8 +2785,8 @@
       <c r="E20" t="s">
         <v>69</v>
       </c>
-      <c r="F20" t="s">
-        <v>70</v>
+      <c r="F20">
+        <v>10</v>
       </c>
       <c r="G20" t="s">
         <v>71</v>
@@ -2815,7 +2821,7 @@
         <v>231</v>
       </c>
       <c r="C21">
-        <v>999</v>
+        <v>18.2</v>
       </c>
       <c r="D21" t="s">
         <v>86</v>
@@ -2823,8 +2829,8 @@
       <c r="E21" t="s">
         <v>69</v>
       </c>
-      <c r="F21" t="s">
-        <v>70</v>
+      <c r="F21">
+        <v>10</v>
       </c>
       <c r="G21" t="s">
         <v>71</v>
@@ -2859,7 +2865,7 @@
         <v>232</v>
       </c>
       <c r="C22">
-        <v>999</v>
+        <v>18.2</v>
       </c>
       <c r="D22" t="s">
         <v>86</v>
@@ -2867,8 +2873,8 @@
       <c r="E22" t="s">
         <v>69</v>
       </c>
-      <c r="F22" t="s">
-        <v>70</v>
+      <c r="F22">
+        <v>10</v>
       </c>
       <c r="G22" t="s">
         <v>71</v>
@@ -2903,7 +2909,7 @@
         <v>96</v>
       </c>
       <c r="C23">
-        <v>999</v>
+        <v>24.8</v>
       </c>
       <c r="D23" t="s">
         <v>86</v>
@@ -2911,8 +2917,8 @@
       <c r="E23" t="s">
         <v>69</v>
       </c>
-      <c r="F23" t="s">
-        <v>70</v>
+      <c r="F23">
+        <v>10</v>
       </c>
       <c r="G23" t="s">
         <v>71</v>
@@ -2947,7 +2953,7 @@
         <v>98</v>
       </c>
       <c r="C24">
-        <v>999</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="D24" t="s">
         <v>86</v>
@@ -2955,8 +2961,8 @@
       <c r="E24" t="s">
         <v>69</v>
       </c>
-      <c r="F24" t="s">
-        <v>70</v>
+      <c r="F24">
+        <v>10</v>
       </c>
       <c r="G24" t="s">
         <v>71</v>
@@ -2991,7 +2997,7 @@
         <v>100</v>
       </c>
       <c r="C25">
-        <v>999</v>
+        <v>483.6</v>
       </c>
       <c r="D25" t="s">
         <v>101</v>
@@ -2999,8 +3005,8 @@
       <c r="E25" t="s">
         <v>69</v>
       </c>
-      <c r="F25" t="s">
-        <v>70</v>
+      <c r="F25">
+        <v>10</v>
       </c>
       <c r="G25" t="s">
         <v>71</v>
@@ -3035,7 +3041,7 @@
         <v>103</v>
       </c>
       <c r="C26">
-        <v>999</v>
+        <v>36</v>
       </c>
       <c r="D26" t="s">
         <v>101</v>
@@ -3043,8 +3049,8 @@
       <c r="E26" t="s">
         <v>69</v>
       </c>
-      <c r="F26" t="s">
-        <v>70</v>
+      <c r="F26">
+        <v>10</v>
       </c>
       <c r="G26" t="s">
         <v>71</v>
@@ -3079,7 +3085,7 @@
         <v>105</v>
       </c>
       <c r="C27">
-        <v>999</v>
+        <v>68.5</v>
       </c>
       <c r="D27" t="s">
         <v>106</v>
@@ -3087,8 +3093,8 @@
       <c r="E27" t="s">
         <v>69</v>
       </c>
-      <c r="F27" t="s">
-        <v>70</v>
+      <c r="F27">
+        <v>15</v>
       </c>
       <c r="G27" t="s">
         <v>71</v>
@@ -3123,7 +3129,7 @@
         <v>108</v>
       </c>
       <c r="C28">
-        <v>999</v>
+        <v>209.7</v>
       </c>
       <c r="D28" t="s">
         <v>109</v>
@@ -3131,8 +3137,8 @@
       <c r="E28" t="s">
         <v>69</v>
       </c>
-      <c r="F28" t="s">
-        <v>70</v>
+      <c r="F28">
+        <v>10</v>
       </c>
       <c r="G28" t="s">
         <v>71</v>
@@ -3167,7 +3173,7 @@
         <v>111</v>
       </c>
       <c r="C29">
-        <v>999</v>
+        <v>209.7</v>
       </c>
       <c r="D29" t="s">
         <v>109</v>
@@ -3175,8 +3181,8 @@
       <c r="E29" t="s">
         <v>69</v>
       </c>
-      <c r="F29" t="s">
-        <v>70</v>
+      <c r="F29">
+        <v>10</v>
       </c>
       <c r="G29" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
[4-3782][1.0.2] software update (#11)
* update codesys project

* update sd card settings

* backup save

* in progress save

* update sd settings

* add new ver screenshots

* update alarm list

* update version

* adjust project name in info page

* update
</commit_message>
<xml_diff>
--- a/4-3782/sd/sd.xlsx
+++ b/4-3782/sd/sd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kordianpiduch/Desktop/4-3782/sd/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kordianpiduch/Desktop/untitled folder/sd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE19F2A-D5E3-2548-BE28-E4FAD3968039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5641B7D5-07C5-6448-ABA2-B87DBCC46E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30080" windowHeight="32120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="37540" windowHeight="27060" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valves" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="232">
   <si>
     <t>filename</t>
   </si>
@@ -243,9 +243,6 @@
   </si>
   <si>
     <t>1025</t>
-  </si>
-  <si>
-    <t>800</t>
   </si>
   <si>
     <t>10</t>
@@ -1106,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1146,7 +1143,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -1160,7 +1157,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -1174,7 +1171,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -1188,7 +1185,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -1202,7 +1199,7 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -1216,7 +1213,7 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -1230,7 +1227,7 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -1244,7 +1241,7 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -1262,7 +1259,7 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1270,7 +1267,7 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -1288,7 +1285,7 @@
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1296,7 +1293,7 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -1310,7 +1307,7 @@
         <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -1324,7 +1321,7 @@
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
@@ -1338,7 +1335,7 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
@@ -1352,7 +1349,7 @@
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
@@ -1366,7 +1363,7 @@
         <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
@@ -1380,7 +1377,7 @@
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
@@ -1394,7 +1391,7 @@
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
@@ -1408,7 +1405,7 @@
         <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
@@ -1422,7 +1419,7 @@
         <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
@@ -1436,7 +1433,7 @@
         <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
@@ -1450,7 +1447,7 @@
         <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
@@ -1464,7 +1461,7 @@
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
@@ -1478,7 +1475,7 @@
         <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
@@ -1492,7 +1489,7 @@
         <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
@@ -1506,7 +1503,7 @@
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
@@ -1520,7 +1517,7 @@
         <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
@@ -1534,7 +1531,7 @@
         <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
@@ -1548,7 +1545,7 @@
         <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
@@ -1562,7 +1559,7 @@
         <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C30" t="s">
         <v>9</v>
@@ -1576,7 +1573,7 @@
         <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C31" t="s">
         <v>9</v>
@@ -1590,7 +1587,7 @@
         <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C32" t="s">
         <v>9</v>
@@ -1604,7 +1601,7 @@
         <v>42</v>
       </c>
       <c r="B33" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C33" t="s">
         <v>9</v>
@@ -1618,7 +1615,7 @@
         <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C34" t="s">
         <v>9</v>
@@ -1632,7 +1629,7 @@
         <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C35" t="s">
         <v>9</v>
@@ -1646,7 +1643,7 @@
         <v>45</v>
       </c>
       <c r="B36" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C36" t="s">
         <v>9</v>
@@ -1660,7 +1657,7 @@
         <v>46</v>
       </c>
       <c r="B37" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C37" t="s">
         <v>9</v>
@@ -1674,7 +1671,7 @@
         <v>47</v>
       </c>
       <c r="B38" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C38" t="s">
         <v>9</v>
@@ -1688,7 +1685,7 @@
         <v>48</v>
       </c>
       <c r="B39" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C39" t="s">
         <v>9</v>
@@ -1702,7 +1699,7 @@
         <v>49</v>
       </c>
       <c r="B40" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C40" t="s">
         <v>9</v>
@@ -1716,7 +1713,7 @@
         <v>50</v>
       </c>
       <c r="B41" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C41" t="s">
         <v>9</v>
@@ -1730,7 +1727,7 @@
         <v>51</v>
       </c>
       <c r="B42" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C42" t="s">
         <v>9</v>
@@ -1744,7 +1741,7 @@
         <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C43" t="s">
         <v>9</v>
@@ -1758,7 +1755,7 @@
         <v>53</v>
       </c>
       <c r="B44" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C44" t="s">
         <v>9</v>
@@ -1772,7 +1769,7 @@
         <v>54</v>
       </c>
       <c r="B45" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C45" t="s">
         <v>9</v>
@@ -1783,10 +1780,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B46" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C46" t="s">
         <v>9</v>
@@ -1797,10 +1794,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B47" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C47" t="s">
         <v>9</v>
@@ -1811,10 +1808,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B48" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C48" t="s">
         <v>9</v>
@@ -1825,10 +1822,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B49" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C49" t="s">
         <v>9</v>
@@ -1839,10 +1836,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B50" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C50" t="s">
         <v>9</v>
@@ -1853,10 +1850,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B51" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C51" t="s">
         <v>9</v>
@@ -1867,10 +1864,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B52" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C52" t="s">
         <v>9</v>
@@ -1881,10 +1878,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B53" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C53" t="s">
         <v>9</v>
@@ -1895,10 +1892,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B54" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C54" t="s">
         <v>9</v>
@@ -1917,14 +1914,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="26.83203125" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" customWidth="1"/>
     <col min="10" max="10" width="21.5" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
@@ -1976,1231 +1979,1231 @@
         <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C2">
-        <v>999</v>
+        <v>1307.7</v>
       </c>
       <c r="D2" t="s">
         <v>68</v>
       </c>
-      <c r="E2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E2">
+        <v>3350</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
         <v>70</v>
       </c>
-      <c r="G2" t="s">
-        <v>71</v>
-      </c>
       <c r="H2" t="s">
         <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J2">
         <v>20.975000000000001</v>
       </c>
       <c r="K2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M2" t="s">
         <v>10</v>
       </c>
       <c r="N2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C3">
-        <v>999</v>
+        <v>1307.7</v>
       </c>
       <c r="D3" t="s">
         <v>68</v>
       </c>
-      <c r="E3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="E3">
+        <v>3350</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
         <v>70</v>
       </c>
-      <c r="G3" t="s">
-        <v>71</v>
-      </c>
       <c r="H3" t="s">
         <v>10</v>
       </c>
       <c r="I3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J3">
         <v>20.975000000000001</v>
       </c>
       <c r="K3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M3" t="s">
         <v>10</v>
       </c>
       <c r="N3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C4">
-        <v>999</v>
+        <v>1737.6</v>
       </c>
       <c r="D4" t="s">
         <v>68</v>
       </c>
-      <c r="E4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="E4">
+        <v>3350</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
         <v>70</v>
       </c>
-      <c r="G4" t="s">
-        <v>71</v>
-      </c>
       <c r="H4" t="s">
         <v>10</v>
       </c>
       <c r="I4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J4">
         <v>20.975000000000001</v>
       </c>
       <c r="K4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M4" t="s">
         <v>10</v>
       </c>
       <c r="N4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C5">
-        <v>999</v>
+        <v>1737.6</v>
       </c>
       <c r="D5" t="s">
         <v>68</v>
       </c>
-      <c r="E5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="E5">
+        <v>3350</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
         <v>70</v>
       </c>
-      <c r="G5" t="s">
-        <v>71</v>
-      </c>
       <c r="H5" t="s">
         <v>10</v>
       </c>
       <c r="I5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J5">
         <v>20.975000000000001</v>
       </c>
       <c r="K5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M5" t="s">
         <v>10</v>
       </c>
       <c r="N5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C6">
-        <v>999</v>
+        <v>3169.1</v>
       </c>
       <c r="D6" t="s">
         <v>68</v>
       </c>
-      <c r="E6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="E6">
+        <v>3350</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
         <v>70</v>
       </c>
-      <c r="G6" t="s">
-        <v>71</v>
-      </c>
       <c r="H6" t="s">
         <v>10</v>
       </c>
       <c r="I6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J6">
         <v>20.975000000000001</v>
       </c>
       <c r="K6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M6" t="s">
         <v>10</v>
       </c>
       <c r="N6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C7">
-        <v>999</v>
+        <v>3169.1</v>
       </c>
       <c r="D7" t="s">
         <v>68</v>
       </c>
-      <c r="E7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="E7">
+        <v>3350</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
         <v>70</v>
       </c>
-      <c r="G7" t="s">
-        <v>71</v>
-      </c>
       <c r="H7" t="s">
         <v>10</v>
       </c>
       <c r="I7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J7">
         <v>20.975000000000001</v>
       </c>
       <c r="K7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M7" t="s">
         <v>10</v>
       </c>
       <c r="N7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C8">
-        <v>999</v>
+        <v>3149.6</v>
       </c>
       <c r="D8" t="s">
         <v>68</v>
       </c>
-      <c r="E8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="E8">
+        <v>3350</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
         <v>70</v>
       </c>
-      <c r="G8" t="s">
-        <v>71</v>
-      </c>
       <c r="H8" t="s">
         <v>10</v>
       </c>
       <c r="I8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J8">
         <v>20.975000000000001</v>
       </c>
       <c r="K8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M8" t="s">
         <v>10</v>
       </c>
       <c r="N8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C9">
-        <v>999</v>
+        <v>3222.9</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
       </c>
-      <c r="E9" t="s">
-        <v>69</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="E9">
+        <v>3350</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
         <v>70</v>
       </c>
-      <c r="G9" t="s">
-        <v>71</v>
-      </c>
       <c r="H9" t="s">
         <v>10</v>
       </c>
       <c r="I9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J9">
         <v>20.975000000000001</v>
       </c>
       <c r="K9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M9" t="s">
         <v>10</v>
       </c>
       <c r="N9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C10">
-        <v>999</v>
+        <v>839.5</v>
       </c>
       <c r="D10" t="s">
         <v>68</v>
       </c>
-      <c r="E10" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="E10">
+        <v>2100</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
         <v>70</v>
       </c>
-      <c r="G10" t="s">
-        <v>71</v>
-      </c>
       <c r="H10" t="s">
         <v>10</v>
       </c>
       <c r="I10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J10">
         <v>7.6189999999999998</v>
       </c>
       <c r="K10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M10" t="s">
         <v>10</v>
       </c>
       <c r="N10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C11">
-        <v>999</v>
+        <v>839.5</v>
       </c>
       <c r="D11" t="s">
         <v>68</v>
       </c>
-      <c r="E11" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="E11">
+        <v>2100</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
         <v>70</v>
       </c>
-      <c r="G11" t="s">
-        <v>71</v>
-      </c>
       <c r="H11" t="s">
         <v>10</v>
       </c>
       <c r="I11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J11">
         <v>7.6189999999999998</v>
       </c>
       <c r="K11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M11" t="s">
         <v>10</v>
       </c>
       <c r="N11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C12">
-        <v>999</v>
+        <v>1508.4</v>
       </c>
       <c r="D12" t="s">
         <v>68</v>
       </c>
-      <c r="E12" t="s">
-        <v>69</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="E12">
+        <v>2300</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
         <v>70</v>
       </c>
-      <c r="G12" t="s">
-        <v>71</v>
-      </c>
       <c r="H12" t="s">
         <v>10</v>
       </c>
       <c r="I12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J12">
         <v>9.3000000000000007</v>
       </c>
       <c r="K12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M12" t="s">
         <v>10</v>
       </c>
       <c r="N12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C13">
-        <v>999</v>
+        <v>661.7</v>
       </c>
       <c r="D13" t="s">
         <v>68</v>
       </c>
-      <c r="E13" t="s">
-        <v>69</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="E13">
+        <v>1863</v>
+      </c>
+      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="G13" t="s">
         <v>70</v>
       </c>
-      <c r="G13" t="s">
-        <v>71</v>
-      </c>
       <c r="H13" t="s">
         <v>10</v>
       </c>
       <c r="I13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J13">
         <v>6.1890000000000001</v>
       </c>
       <c r="K13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M13" t="s">
         <v>10</v>
       </c>
       <c r="N13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" t="s">
+        <v>213</v>
+      </c>
+      <c r="C14">
+        <v>396.5</v>
+      </c>
+      <c r="D14" t="s">
         <v>85</v>
       </c>
-      <c r="B14" t="s">
-        <v>214</v>
-      </c>
-      <c r="C14">
-        <v>999</v>
-      </c>
-      <c r="D14" t="s">
-        <v>86</v>
-      </c>
-      <c r="E14" t="s">
-        <v>69</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="E14">
+        <v>1700</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
         <v>70</v>
       </c>
-      <c r="G14" t="s">
-        <v>71</v>
-      </c>
       <c r="H14" t="s">
         <v>10</v>
       </c>
       <c r="I14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J14">
         <v>4.7519999999999998</v>
       </c>
       <c r="K14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M14" t="s">
         <v>10</v>
       </c>
       <c r="N14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C15">
-        <v>999</v>
+        <v>631.29999999999995</v>
       </c>
       <c r="D15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E15" t="s">
-        <v>69</v>
-      </c>
-      <c r="F15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15">
+        <v>1688</v>
+      </c>
+      <c r="F15">
+        <v>10</v>
+      </c>
+      <c r="G15" t="s">
         <v>70</v>
       </c>
-      <c r="G15" t="s">
-        <v>71</v>
-      </c>
       <c r="H15" t="s">
         <v>10</v>
       </c>
       <c r="I15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J15">
         <v>4.7519999999999998</v>
       </c>
       <c r="K15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M15" t="s">
         <v>10</v>
       </c>
       <c r="N15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C16">
-        <v>999</v>
+        <v>308.2</v>
       </c>
       <c r="D16" t="s">
-        <v>86</v>
-      </c>
-      <c r="E16" t="s">
-        <v>69</v>
-      </c>
-      <c r="F16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16">
+        <v>1688</v>
+      </c>
+      <c r="F16">
+        <v>10</v>
+      </c>
+      <c r="G16" t="s">
         <v>70</v>
       </c>
-      <c r="G16" t="s">
-        <v>71</v>
-      </c>
       <c r="H16" t="s">
         <v>10</v>
       </c>
       <c r="I16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J16">
         <v>4.7519999999999998</v>
       </c>
       <c r="K16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M16" t="s">
         <v>10</v>
       </c>
       <c r="N16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C17">
-        <v>999</v>
+        <v>367.3</v>
       </c>
       <c r="D17" t="s">
-        <v>86</v>
-      </c>
-      <c r="E17" t="s">
-        <v>69</v>
-      </c>
-      <c r="F17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17">
+        <v>1828</v>
+      </c>
+      <c r="F17">
+        <v>10</v>
+      </c>
+      <c r="G17" t="s">
         <v>70</v>
       </c>
-      <c r="G17" t="s">
-        <v>71</v>
-      </c>
       <c r="H17" t="s">
         <v>10</v>
       </c>
       <c r="I17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J17">
         <v>6.21</v>
       </c>
       <c r="K17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M17" t="s">
         <v>10</v>
       </c>
       <c r="N17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C18">
-        <v>999</v>
+        <v>264.39999999999998</v>
       </c>
       <c r="D18" t="s">
-        <v>86</v>
-      </c>
-      <c r="E18" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18">
+        <v>1707</v>
+      </c>
+      <c r="F18">
+        <v>10</v>
+      </c>
+      <c r="G18" t="s">
         <v>70</v>
       </c>
-      <c r="G18" t="s">
-        <v>71</v>
-      </c>
       <c r="H18" t="s">
         <v>10</v>
       </c>
       <c r="I18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J18">
         <v>4.95</v>
       </c>
       <c r="K18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M18" t="s">
         <v>10</v>
       </c>
       <c r="N18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C19">
-        <v>999</v>
+        <v>24.2</v>
       </c>
       <c r="D19" t="s">
-        <v>86</v>
-      </c>
-      <c r="E19" t="s">
-        <v>69</v>
-      </c>
-      <c r="F19" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19">
+        <v>1736</v>
+      </c>
+      <c r="F19">
+        <v>10</v>
+      </c>
+      <c r="G19" t="s">
         <v>70</v>
       </c>
-      <c r="G19" t="s">
-        <v>71</v>
-      </c>
       <c r="H19" t="s">
         <v>10</v>
       </c>
       <c r="I19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J19">
         <v>5.25</v>
       </c>
       <c r="K19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M19" t="s">
         <v>10</v>
       </c>
       <c r="N19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C20">
-        <v>999</v>
+        <v>24.2</v>
       </c>
       <c r="D20" t="s">
-        <v>86</v>
-      </c>
-      <c r="E20" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20">
+        <v>1736</v>
+      </c>
+      <c r="F20">
+        <v>10</v>
+      </c>
+      <c r="G20" t="s">
         <v>70</v>
       </c>
-      <c r="G20" t="s">
-        <v>71</v>
-      </c>
       <c r="H20" t="s">
         <v>10</v>
       </c>
       <c r="I20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J20">
         <v>5.25</v>
       </c>
       <c r="K20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M20" t="s">
         <v>10</v>
       </c>
       <c r="N20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B21" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C21">
-        <v>999</v>
+        <v>18.2</v>
       </c>
       <c r="D21" t="s">
-        <v>86</v>
-      </c>
-      <c r="E21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F21" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21">
+        <v>1736</v>
+      </c>
+      <c r="F21">
+        <v>10</v>
+      </c>
+      <c r="G21" t="s">
         <v>70</v>
       </c>
-      <c r="G21" t="s">
-        <v>71</v>
-      </c>
       <c r="H21" t="s">
         <v>10</v>
       </c>
       <c r="I21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J21">
         <v>5.25</v>
       </c>
       <c r="K21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M21" t="s">
         <v>10</v>
       </c>
       <c r="N21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C22">
-        <v>999</v>
+        <v>18.2</v>
       </c>
       <c r="D22" t="s">
-        <v>86</v>
-      </c>
-      <c r="E22" t="s">
-        <v>69</v>
-      </c>
-      <c r="F22" t="s">
+        <v>85</v>
+      </c>
+      <c r="E22">
+        <v>1736</v>
+      </c>
+      <c r="F22">
+        <v>10</v>
+      </c>
+      <c r="G22" t="s">
         <v>70</v>
       </c>
-      <c r="G22" t="s">
-        <v>71</v>
-      </c>
       <c r="H22" t="s">
         <v>10</v>
       </c>
       <c r="I22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J22">
         <v>5.25</v>
       </c>
       <c r="K22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M22" t="s">
         <v>10</v>
       </c>
       <c r="N22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B23" t="s">
         <v>95</v>
       </c>
-      <c r="B23" t="s">
-        <v>96</v>
-      </c>
       <c r="C23">
-        <v>999</v>
+        <v>24.8</v>
       </c>
       <c r="D23" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23" t="s">
-        <v>69</v>
-      </c>
-      <c r="F23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23">
+        <v>1460</v>
+      </c>
+      <c r="F23">
+        <v>10</v>
+      </c>
+      <c r="G23" t="s">
         <v>70</v>
       </c>
-      <c r="G23" t="s">
-        <v>71</v>
-      </c>
       <c r="H23" t="s">
         <v>10</v>
       </c>
       <c r="I23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J23">
         <v>2.36</v>
       </c>
       <c r="K23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M23" t="s">
         <v>10</v>
       </c>
       <c r="N23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" t="s">
         <v>97</v>
       </c>
-      <c r="B24" t="s">
-        <v>98</v>
-      </c>
       <c r="C24">
-        <v>999</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="D24" t="s">
-        <v>86</v>
-      </c>
-      <c r="E24" t="s">
-        <v>69</v>
-      </c>
-      <c r="F24" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24">
+        <v>1460</v>
+      </c>
+      <c r="F24">
+        <v>10</v>
+      </c>
+      <c r="G24" t="s">
         <v>70</v>
       </c>
-      <c r="G24" t="s">
-        <v>71</v>
-      </c>
       <c r="H24" t="s">
         <v>10</v>
       </c>
       <c r="I24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J24">
         <v>2.36</v>
       </c>
       <c r="K24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M24" t="s">
         <v>10</v>
       </c>
       <c r="N24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" t="s">
         <v>99</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25">
+        <v>483.6</v>
+      </c>
+      <c r="D25" t="s">
         <v>100</v>
       </c>
-      <c r="C25">
-        <v>999</v>
-      </c>
-      <c r="D25" t="s">
-        <v>101</v>
-      </c>
-      <c r="E25" t="s">
-        <v>69</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="E25">
+        <v>2155</v>
+      </c>
+      <c r="F25">
+        <v>10</v>
+      </c>
+      <c r="G25" t="s">
         <v>70</v>
       </c>
-      <c r="G25" t="s">
-        <v>71</v>
-      </c>
       <c r="H25" t="s">
         <v>10</v>
       </c>
       <c r="I25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J25">
         <v>11.05</v>
       </c>
       <c r="K25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M25" t="s">
         <v>10</v>
       </c>
       <c r="N25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" t="s">
         <v>102</v>
       </c>
-      <c r="B26" t="s">
-        <v>103</v>
-      </c>
       <c r="C26">
-        <v>999</v>
+        <v>36</v>
       </c>
       <c r="D26" t="s">
-        <v>101</v>
-      </c>
-      <c r="E26" t="s">
-        <v>69</v>
-      </c>
-      <c r="F26" t="s">
+        <v>100</v>
+      </c>
+      <c r="E26">
+        <v>1736</v>
+      </c>
+      <c r="F26">
+        <v>10</v>
+      </c>
+      <c r="G26" t="s">
         <v>70</v>
       </c>
-      <c r="G26" t="s">
-        <v>71</v>
-      </c>
       <c r="H26" t="s">
         <v>10</v>
       </c>
       <c r="I26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J26">
         <v>6.1</v>
       </c>
       <c r="K26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M26" t="s">
         <v>10</v>
       </c>
       <c r="N26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" t="s">
         <v>104</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27">
+        <v>68.5</v>
+      </c>
+      <c r="D27" t="s">
         <v>105</v>
       </c>
-      <c r="C27">
-        <v>999</v>
-      </c>
-      <c r="D27" t="s">
-        <v>106</v>
-      </c>
-      <c r="E27" t="s">
-        <v>69</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="E27">
+        <v>1728</v>
+      </c>
+      <c r="F27">
+        <v>15</v>
+      </c>
+      <c r="G27" t="s">
         <v>70</v>
       </c>
-      <c r="G27" t="s">
-        <v>71</v>
-      </c>
       <c r="H27" t="s">
         <v>10</v>
       </c>
       <c r="I27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J27">
         <v>3.45</v>
       </c>
       <c r="K27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M27" t="s">
         <v>10</v>
       </c>
       <c r="N27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" t="s">
         <v>107</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28">
+        <v>209.7</v>
+      </c>
+      <c r="D28" t="s">
         <v>108</v>
       </c>
-      <c r="C28">
-        <v>999</v>
-      </c>
-      <c r="D28" t="s">
-        <v>109</v>
-      </c>
-      <c r="E28" t="s">
-        <v>69</v>
-      </c>
-      <c r="F28" t="s">
+      <c r="E28">
+        <v>1865</v>
+      </c>
+      <c r="F28">
+        <v>10</v>
+      </c>
+      <c r="G28" t="s">
         <v>70</v>
       </c>
-      <c r="G28" t="s">
-        <v>71</v>
-      </c>
       <c r="H28" t="s">
         <v>10</v>
       </c>
       <c r="I28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J28">
         <v>6.4</v>
       </c>
       <c r="K28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M28" t="s">
         <v>10</v>
       </c>
       <c r="N28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" t="s">
         <v>110</v>
       </c>
-      <c r="B29" t="s">
-        <v>111</v>
-      </c>
       <c r="C29">
-        <v>999</v>
+        <v>209.7</v>
       </c>
       <c r="D29" t="s">
-        <v>109</v>
-      </c>
-      <c r="E29" t="s">
-        <v>69</v>
-      </c>
-      <c r="F29" t="s">
+        <v>108</v>
+      </c>
+      <c r="E29">
+        <v>1865</v>
+      </c>
+      <c r="F29">
+        <v>10</v>
+      </c>
+      <c r="G29" t="s">
         <v>70</v>
       </c>
-      <c r="G29" t="s">
-        <v>71</v>
-      </c>
       <c r="H29" t="s">
         <v>10</v>
       </c>
       <c r="I29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J29">
         <v>6.4</v>
       </c>
       <c r="K29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M29" t="s">
         <v>10</v>
       </c>
       <c r="N29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -3229,91 +3232,91 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C2" t="s">
         <v>119</v>
       </c>
-      <c r="B2" t="s">
-        <v>227</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
         <v>120</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
         <v>121</v>
       </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>122</v>
-      </c>
       <c r="H2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C3" t="s">
         <v>123</v>
       </c>
-      <c r="B3" t="s">
-        <v>228</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>124</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>125</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>126</v>
       </c>
-      <c r="F3" t="s">
-        <v>127</v>
-      </c>
       <c r="G3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>218</v>
+      </c>
+      <c r="B4" t="s">
         <v>219</v>
-      </c>
-      <c r="B4" t="s">
-        <v>220</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -3339,10 +3342,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B5" t="s">
         <v>221</v>
-      </c>
-      <c r="B5" t="s">
-        <v>222</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -3368,10 +3371,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>222</v>
+      </c>
+      <c r="B6" t="s">
         <v>223</v>
-      </c>
-      <c r="B6" t="s">
-        <v>224</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -3397,10 +3400,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>224</v>
+      </c>
+      <c r="B7" t="s">
         <v>225</v>
-      </c>
-      <c r="B7" t="s">
-        <v>226</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -3433,8 +3436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3447,7 +3450,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>56</v>
@@ -3459,15 +3462,15 @@
         <v>58</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" t="s">
         <v>130</v>
-      </c>
-      <c r="B2" t="s">
-        <v>131</v>
       </c>
       <c r="C2">
         <v>14.5</v>
@@ -3476,21 +3479,21 @@
         <v>68</v>
       </c>
       <c r="E2">
-        <v>800</v>
+        <v>2700</v>
       </c>
       <c r="F2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" t="s">
         <v>133</v>
-      </c>
-      <c r="B3" t="s">
-        <v>134</v>
       </c>
       <c r="C3">
         <v>14.5</v>
@@ -3499,21 +3502,21 @@
         <v>68</v>
       </c>
       <c r="E3">
-        <v>800</v>
+        <v>2700</v>
       </c>
       <c r="F3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" t="s">
         <v>135</v>
-      </c>
-      <c r="B4" t="s">
-        <v>136</v>
       </c>
       <c r="C4">
         <v>14.5</v>
@@ -3522,21 +3525,21 @@
         <v>68</v>
       </c>
       <c r="E4">
-        <v>800</v>
+        <v>2700</v>
       </c>
       <c r="F4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" t="s">
         <v>137</v>
-      </c>
-      <c r="B5" t="s">
-        <v>138</v>
       </c>
       <c r="C5">
         <v>14.5</v>
@@ -3545,13 +3548,13 @@
         <v>68</v>
       </c>
       <c r="E5">
-        <v>800</v>
+        <v>2700</v>
       </c>
       <c r="F5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>